<commit_message>
Slight changes to calculator
</commit_message>
<xml_diff>
--- a/EE/Maths/theBigBatteryCalculator.xlsx
+++ b/EE/Maths/theBigBatteryCalculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\StormDrainRobot\EE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evere\Documents\GitHub\StormDrainRobot\EE\Maths\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6F5C0A-CA16-46CB-BCBC-4FB243013932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03F8AC0-46E5-4024-9482-2C1EECAB5CA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2805E8E7-BA38-41BF-957C-17387B357D35}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="1" xr2:uid="{2805E8E7-BA38-41BF-957C-17387B357D35}"/>
   </bookViews>
   <sheets>
     <sheet name="TBDraw" sheetId="1" r:id="rId1"/>
@@ -388,6 +388,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -395,12 +401,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -722,42 +722,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE54EED-B1A0-4032-9FB8-85DBBA9E4F32}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.3984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
         <v>28</v>
@@ -790,7 +790,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -837,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -885,7 +885,7 @@
         <v>0.1010507575186637</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
@@ -926,7 +926,7 @@
         <v>4.1279999999999997E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
@@ -966,7 +966,7 @@
         <v>51.84</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
         <v>10</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="10" t="s">
         <v>51</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
         <v>50</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="10" t="s">
         <v>12</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
         <v>13</v>
       </c>
@@ -1207,14 +1207,14 @@
         <v>58.205236330750289</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="24">
         <v>4</v>
       </c>
       <c r="D13" s="3">
@@ -1247,7 +1247,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
         <v>15</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
         <v>16</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>2.4000000000000002E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
         <v>17</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>0.22799999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1427,7 +1427,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="12"/>
       <c r="B19" s="4"/>
       <c r="J19" s="8">
@@ -1438,7 +1438,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="J20" s="2">
         <f>Sources!G2/SUM(K3:K17)</f>
         <v>1.6296482483247907</v>
@@ -1461,43 +1461,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C451F7D-53A0-4E77-A790-BDC17E7586E6}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="C8:F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.73046875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
       <c r="J1" s="29"/>
-      <c r="K1" s="28"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K1" s="25"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="9"/>
       <c r="B2" s="3" t="s">
         <v>28</v>
@@ -1537,7 +1537,7 @@
         <v>0.1010507575186637</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>19.200000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1637,15 +1637,15 @@
         <v>0.75</v>
       </c>
       <c r="F5" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="2"/>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="I5" s="3">
         <f>0.1</f>
@@ -1653,14 +1653,14 @@
       </c>
       <c r="J5" s="21">
         <f t="shared" si="3"/>
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="K5" s="21">
         <f t="shared" si="4"/>
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>1.7999999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="1"/>
@@ -1740,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>29.102618165375144</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="10" t="s">
         <v>14</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1873,27 +1873,27 @@
       <c r="H11" s="13"/>
       <c r="J11" s="8">
         <f>SUM(J3:J10)</f>
-        <v>6.5276090902239643</v>
+        <v>6.5126090902239646</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="12"/>
       <c r="B12" s="4"/>
       <c r="J12" s="18">
-        <f>Sources!F3/TGDraw!J11</f>
-        <v>1.3787590334535806</v>
+        <f>2*Sources!F3/TGDraw!J11</f>
+        <v>2.7638692497327506</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="J13" s="2">
         <f>SUM(K3:K10)/Sources!G3</f>
-        <v>0.51750077232271341</v>
+        <v>0.51701057624428204</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>53</v>
@@ -1915,18 +1915,18 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>7</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>2.748893571891069</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>250</v>
       </c>
@@ -2012,17 +2012,17 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>

</xml_diff>